<commit_message>
add chart excel doctor
</commit_message>
<xml_diff>
--- a/doc/Chart Dashboard Healthcare BATS.xlsx
+++ b/doc/Chart Dashboard Healthcare BATS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sistem_internal_bats\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17608145-DCA6-482F-B5A8-4763F9958A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5787B1-14A8-4EA1-B1CB-63957B734736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{82995AAA-A28D-4E77-8683-5EAD1978BB5F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="85">
   <si>
     <t>Jenis</t>
   </si>
@@ -201,24 +201,6 @@
     <t>Jumlah Kunjungan Berdasarkan Jenis Pasien Di Setiap Bulan</t>
   </si>
   <si>
-    <t>Pendapatan dari Pelayanan Dokter</t>
-  </si>
-  <si>
-    <t>Jenis Penjamin yang Paling Sering Digunakan oleh Pasien Setiap Dokter</t>
-  </si>
-  <si>
-    <t>Rata-rata Tarif Dokter</t>
-  </si>
-  <si>
-    <t>Rata-rata Jumlah yang Dibayarkan oleh Penjamin</t>
-  </si>
-  <si>
-    <t>Pembayaran Paling Tertinggi dan Terendah dari Pasien untuk Setiap Dokter:</t>
-  </si>
-  <si>
-    <t>Perbandingan Kinerja Dokter</t>
-  </si>
-  <si>
     <t>fd2</t>
   </si>
   <si>
@@ -246,18 +228,6 @@
     <t>Jumlah Pasien Rawat Inap yang Ditangani oleh Setiap Dokter</t>
   </si>
   <si>
-    <t>Pendapatan dari Pelayanan Dokter untuk Rawat Jalan dan Rawat Inap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pendapatan dari Pelayanan Dokter untuk Rawat Jalan </t>
-  </si>
-  <si>
-    <t>Pendapatan dari Pelayanan Dokter untuk Rawat Inap</t>
-  </si>
-  <si>
-    <t>Jenis Penjamin yang Paling Sering Digunakan oleh Pasien Rawat Jalan dan Rawat Inap Setiap Dokter</t>
-  </si>
-  <si>
     <t>Jumlah Pasien Rawat Jalan dan Rawat Inap yang Ditangani oleh Setiap Dokter berdasarkan jenis pasien.</t>
   </si>
   <si>
@@ -268,6 +238,60 @@
   </si>
   <si>
     <t>Dokter</t>
+  </si>
+  <si>
+    <t>fd9</t>
+  </si>
+  <si>
+    <t>Jumlah Pasien Rawat Inap yang Ditangani oleh Setiap Dokter Berdasarkan Jenis Pasien</t>
+  </si>
+  <si>
+    <t>Jumlah Pasien yang ditangani oleh dokter per Tahun dan Dokter</t>
+  </si>
+  <si>
+    <t>fd10</t>
+  </si>
+  <si>
+    <t>Pendapatan dari Pelayanan Dokter untuk Rawat Jalan dan Rawat Inap Pertahun</t>
+  </si>
+  <si>
+    <t>Pendapatan dari Pelayanan Dokter untuk Rawat Jalan  Pertahun</t>
+  </si>
+  <si>
+    <t>Pendapatan dari Pelayanan Dokter untuk Rawat Inap Pertahun</t>
+  </si>
+  <si>
+    <t>Pendapatan dari Pelayanan Dokter untuk Rawat Jalan dan Rawat Inap Pertahun Berdasarkan Jenis Pasien</t>
+  </si>
+  <si>
+    <t>Pendapatan dari Pelayanan Dokter untuk Rawat Jalan  Pertahun Berdasarkan Jenis Pasien</t>
+  </si>
+  <si>
+    <t>Pendapatan dari Pelayanan Dokter untuk Rawat Inap Pertahun Berdasarkan Jenis Pasien</t>
+  </si>
+  <si>
+    <t>Pendapatan dari Pelayanan Dokter untuk Rawat Jalan dan Rawat Inap per Dokter</t>
+  </si>
+  <si>
+    <t>Pendapatan dari Pelayanan Dokter untuk Rawat Jalan  per Dokter</t>
+  </si>
+  <si>
+    <t>Pendapatan dari Pelayanan Dokter untuk Rawat Inap per Dokter</t>
+  </si>
+  <si>
+    <t>Pendapatan dari Pelayanan Dokter untuk Rawat Jalan Berdasarkan Jenis Pasien per Dokter</t>
+  </si>
+  <si>
+    <t>Pendapatan dari Pelayanan Dokter untuk Rawat Inap Berdasarkan Jenis Pasien per Dokter</t>
+  </si>
+  <si>
+    <t>Pendapatan dari Pelayanan Dokter untuk Rawat Jalan dan Rawat Inap Berdasarkan Jenis Pasien per Dokter</t>
+  </si>
+  <si>
+    <t>Pembayaran Paling Tertinggi dan Terendah dari Pasien untuk  per Dokter</t>
+  </si>
+  <si>
+    <t>Per tahun dulu baru per dokter</t>
   </si>
 </sst>
 </file>
@@ -305,7 +329,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -333,6 +357,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -364,12 +400,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
@@ -392,6 +425,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE5CCFD-3858-4DBD-8B24-C3FE1DAA58B6}">
-  <dimension ref="C5:G51"/>
+  <dimension ref="C5:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -743,537 +778,647 @@
   </cols>
   <sheetData>
     <row r="5" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="3:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>1</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C7" s="12"/>
-      <c r="D7" s="6">
+      <c r="C7" s="11"/>
+      <c r="D7" s="5">
         <v>2</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C8" s="12"/>
-      <c r="D8" s="6">
+      <c r="C8" s="11"/>
+      <c r="D8" s="5">
         <v>3</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C9" s="12"/>
-      <c r="D9" s="6">
+      <c r="C9" s="11"/>
+      <c r="D9" s="5">
         <v>4</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C10" s="12"/>
-      <c r="D10" s="6">
+      <c r="C10" s="11"/>
+      <c r="D10" s="5">
         <v>5</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C11" s="12"/>
-      <c r="D11" s="6">
+      <c r="C11" s="11"/>
+      <c r="D11" s="5">
         <v>6</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C12" s="12"/>
-      <c r="D12" s="6">
+      <c r="C12" s="11"/>
+      <c r="D12" s="5">
         <v>7</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C13" s="12"/>
-      <c r="D13" s="6">
+      <c r="C13" s="11"/>
+      <c r="D13" s="5">
         <v>8</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C14" s="12"/>
-      <c r="D14" s="6">
+      <c r="C14" s="11"/>
+      <c r="D14" s="5">
         <v>9</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C15" s="12"/>
-      <c r="D15" s="6">
+      <c r="C15" s="11"/>
+      <c r="D15" s="5">
         <v>10</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C16" s="12"/>
-      <c r="D16" s="6">
-        <v>11</v>
-      </c>
-      <c r="E16" s="9" t="s">
+      <c r="C16" s="11"/>
+      <c r="D16" s="5">
+        <v>11</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C17" s="12"/>
-      <c r="D17" s="6">
+      <c r="C17" s="11"/>
+      <c r="D17" s="5">
         <v>12</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C18" s="12"/>
-      <c r="D18" s="6">
+      <c r="C18" s="11"/>
+      <c r="D18" s="5">
         <v>13</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C19" s="12"/>
-      <c r="D19" s="6">
+      <c r="C19" s="11"/>
+      <c r="D19" s="5">
         <v>14</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C20" s="12"/>
-      <c r="D20" s="6">
+      <c r="C20" s="11"/>
+      <c r="D20" s="5">
         <v>15</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C21" s="12"/>
-      <c r="D21" s="6">
+      <c r="C21" s="11"/>
+      <c r="D21" s="5">
         <v>16</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C22" s="12"/>
-      <c r="D22" s="6">
+      <c r="C22" s="11"/>
+      <c r="D22" s="5">
         <v>17</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="G22" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C23" s="12"/>
-      <c r="D23" s="6">
+      <c r="C23" s="11"/>
+      <c r="D23" s="5">
         <v>18</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="G23" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C24" s="12"/>
-      <c r="D24" s="6">
+      <c r="C24" s="11"/>
+      <c r="D24" s="5">
         <v>19</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G24" s="11"/>
+      <c r="G24" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C25" s="12"/>
-      <c r="D25" s="6">
+      <c r="C25" s="11"/>
+      <c r="D25" s="5">
         <v>20</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G25" s="11"/>
+      <c r="G25" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C26" s="12"/>
-      <c r="D26" s="6">
+      <c r="C26" s="11"/>
+      <c r="D26" s="5">
         <v>21</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G26" s="8" t="s">
+      <c r="G26" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C27" s="12"/>
-      <c r="D27" s="6">
+      <c r="C27" s="11"/>
+      <c r="D27" s="5">
         <v>22</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G27" s="11"/>
+      <c r="G27" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C28" s="12"/>
-      <c r="D28" s="6">
+      <c r="C28" s="11"/>
+      <c r="D28" s="5">
         <v>23</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="F28" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G28" s="11"/>
+      <c r="G28" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="29" spans="3:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="5">
+        <v>1</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C30" s="11"/>
+      <c r="D30" s="5">
+        <v>2</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C31" s="11"/>
+      <c r="D31" s="5">
+        <v>3</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C32" s="11"/>
+      <c r="D32" s="5">
+        <v>4</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C33" s="11"/>
+      <c r="D33" s="5">
+        <v>5</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I33" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C34" s="11"/>
+      <c r="D34" s="5">
+        <v>6</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C35" s="11"/>
+      <c r="D35" s="5">
+        <v>7</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C36" s="11"/>
+      <c r="D36" s="5">
+        <v>8</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C37" s="11"/>
+      <c r="D37" s="5">
+        <v>9</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C38" s="11"/>
+      <c r="D38" s="5">
+        <v>10</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C39" s="11"/>
+      <c r="D39" s="5">
+        <v>11</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+    </row>
+    <row r="40" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C40" s="11"/>
+      <c r="D40" s="5">
+        <v>12</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+    </row>
+    <row r="41" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C41" s="11"/>
+      <c r="D41" s="5">
+        <v>13</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+    </row>
+    <row r="42" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C42" s="11"/>
+      <c r="D42" s="5">
+        <v>14</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F42" s="5"/>
+      <c r="G42" s="10"/>
+    </row>
+    <row r="43" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C43" s="11"/>
+      <c r="D43" s="5">
+        <v>15</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F43" s="5"/>
+      <c r="G43" s="10"/>
+    </row>
+    <row r="44" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C44" s="11"/>
+      <c r="D44" s="5">
+        <v>16</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F44" s="5"/>
+      <c r="G44" s="10"/>
+    </row>
+    <row r="45" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C45" s="11"/>
+      <c r="D45" s="5">
+        <v>17</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F45" s="5"/>
+      <c r="G45" s="10"/>
+    </row>
+    <row r="46" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C46" s="11"/>
+      <c r="D46" s="5">
+        <v>18</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F46" s="5"/>
+      <c r="G46" s="10"/>
+    </row>
+    <row r="47" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C47" s="11"/>
+      <c r="D47" s="5">
+        <v>19</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F47" s="5"/>
+      <c r="G47" s="10"/>
+    </row>
+    <row r="48" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C48" s="11"/>
+      <c r="D48" s="5">
+        <v>20</v>
+      </c>
+      <c r="E48" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C30" s="12"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C31" s="12"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C32" s="12"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C33" s="12"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="G33" s="11"/>
-    </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C34" s="12"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="G34" s="11"/>
-    </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C35" s="12"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C36" s="12"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="G36" s="11"/>
-    </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C37" s="3"/>
-    </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C38" s="3"/>
-    </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C39" s="3"/>
-    </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C40" s="3"/>
-    </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C41" s="3"/>
-      <c r="E41" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C42" s="3"/>
-      <c r="E42" t="s">
-        <v>54</v>
-      </c>
-      <c r="F42" s="2"/>
-    </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C43" s="3"/>
-      <c r="E43" t="s">
-        <v>55</v>
-      </c>
-      <c r="F43" s="2"/>
-    </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C44" s="3"/>
-      <c r="E44" t="s">
-        <v>56</v>
-      </c>
-      <c r="F44" s="2"/>
-    </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C45" s="3"/>
-      <c r="E45" t="s">
-        <v>57</v>
-      </c>
-      <c r="F45" s="2"/>
-    </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C46" s="3"/>
-      <c r="E46" t="s">
-        <v>58</v>
-      </c>
-      <c r="F46" s="2"/>
-    </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C47" s="3"/>
-      <c r="E47" t="s">
-        <v>59</v>
-      </c>
-      <c r="F47" s="2"/>
-    </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C48" s="3"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C49" s="3"/>
+      <c r="C49" s="2"/>
     </row>
     <row r="50" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C50" s="3"/>
+      <c r="C50" s="2"/>
     </row>
     <row r="51" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C51" s="3"/>
+      <c r="C51" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C6:C28"/>
-    <mergeCell ref="C29:C36"/>
+    <mergeCell ref="C29:C48"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>